<commit_message>
changed sample data and parameters in co2 sea mode
</commit_message>
<xml_diff>
--- a/pyloghub/sample_data/CO2Sea.xlsx
+++ b/pyloghub/sample_data/CO2Sea.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\log-hub-python\pyloghub\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E498343-7B99-4BE5-A55C-5494866F303F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2F86BE-54B5-44F8-9C34-1271CBC38B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0490A7E-4CDC-4B71-9257-3B3249FB2727}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A0490A7E-4CDC-4B71-9257-3B3249FB2727}"/>
   </bookViews>
   <sheets>
     <sheet name="sea" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>shipment_001</t>
   </si>
@@ -47,9 +47,6 @@
     <t>CNSHG</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -140,13 +137,13 @@
     <t>toUnLocode</t>
   </si>
   <si>
-    <t>vesselId</t>
-  </si>
-  <si>
     <t>isRefrigirated</t>
   </si>
   <si>
     <t>weight</t>
+  </si>
+  <si>
+    <t>distance</t>
   </si>
 </sst>
 </file>
@@ -200,11 +197,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -235,8 +233,8 @@
     <tableColumn id="2" xr3:uid="{463C8547-800E-4F1A-8BF0-29642B73EEDF}" name="shipmentDate" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{0C6DF7C1-614B-40B0-93D9-C3ACEC97D1B3}" name="fromUnLocode"/>
     <tableColumn id="4" xr3:uid="{44FE9449-4413-4635-A123-4302CC32313E}" name="toUnLocode"/>
-    <tableColumn id="5" xr3:uid="{5EC7CAF6-7C5E-48BF-AFFB-96C3AB6363FB}" name="vesselId"/>
     <tableColumn id="6" xr3:uid="{3D660837-AEC2-49A6-879C-3B5B344564AE}" name="isRefrigirated"/>
+    <tableColumn id="5" xr3:uid="{C1DFE465-0E8C-4547-9888-18FABD46C485}" name="distance"/>
     <tableColumn id="7" xr3:uid="{58900AFD-AE8C-4AF6-9531-ECE7BE7381E2}" name="weight"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -587,38 +585,38 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -637,19 +635,16 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
       <c r="H2">
         <v>336</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>44837</v>
@@ -658,24 +653,21 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
       </c>
       <c r="H3">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>44837</v>
@@ -684,24 +676,21 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
       </c>
       <c r="H4">
         <v>460</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
         <v>44837</v>
@@ -710,24 +699,21 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>4</v>
       </c>
       <c r="H5">
         <v>360</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
         <v>44838</v>
@@ -736,24 +722,21 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
       </c>
       <c r="H6">
         <v>301</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
         <v>44838</v>
@@ -762,24 +745,21 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
         <v>3</v>
-      </c>
-      <c r="G7" t="s">
-        <v>4</v>
       </c>
       <c r="H7">
         <v>564</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1">
         <v>44839</v>
@@ -788,24 +768,21 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
         <v>3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>4</v>
       </c>
       <c r="H8">
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
         <v>44840</v>
@@ -814,24 +791,21 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
       </c>
       <c r="H9">
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1">
         <v>44840</v>
@@ -840,24 +814,21 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>4</v>
       </c>
       <c r="H10">
         <v>492</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1">
         <v>44840</v>
@@ -866,24 +837,21 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
         <v>3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>4</v>
       </c>
       <c r="H11">
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1">
         <v>44841</v>
@@ -892,24 +860,21 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>4</v>
       </c>
       <c r="H12">
         <v>324</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1">
         <v>44841</v>
@@ -918,24 +883,21 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
         <v>3</v>
-      </c>
-      <c r="G13" t="s">
-        <v>4</v>
       </c>
       <c r="H13">
         <v>454</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1">
         <v>44841</v>
@@ -944,13 +906,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
         <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>4</v>
       </c>
       <c r="H14">
         <v>466</v>

</xml_diff>